<commit_message>
updating arm dxl config pid
</commit_message>
<xml_diff>
--- a/armadillo2_hw/config/manipulatorh_rmanager_config.xlsx
+++ b/armadillo2_hw/config/manipulatorh_rmanager_config.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
   <si>
     <t xml:space="preserve">modor id</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">vel P gain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vel I gain</t>
   </si>
   <si>
     <t xml:space="preserve">h54-200-s500-r/54024</t>
@@ -201,23 +204,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.5587044534413"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.2793522267206"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.8582995951417"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.5303643724696"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.6599190283401"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.4453441295547"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="14.1093117408907"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.7125506072875"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.497975708502"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="1022" min="10" style="1" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.57085020242915"/>
   </cols>
@@ -250,16 +253,19 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>-125475</v>
@@ -268,16 +274,19 @@
         <v>125475</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>250</v>
+        <v>600</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>500</v>
+        <v>700</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -285,10 +294,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>-143930</v>
@@ -297,16 +306,19 @@
         <v>143661</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H3" s="1" t="n">
-        <v>250</v>
+        <v>850</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>500</v>
+        <v>700</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -314,10 +326,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>-121181</v>
@@ -326,16 +338,19 @@
         <v>188612</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>500</v>
+        <v>350</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -343,10 +358,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>-250950</v>
@@ -355,16 +370,19 @@
         <v>250542</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>500</v>
+        <v>350</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -372,10 +390,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>-76574</v>
@@ -384,16 +402,19 @@
         <v>75796</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H6" s="1" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="I6" s="1" t="n">
         <v>440</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -401,10 +422,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>-151900</v>
@@ -413,16 +434,19 @@
         <v>148934</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H7" s="1" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="I7" s="1" t="n">
         <v>440</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -430,7 +454,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>0</v>
@@ -442,7 +466,7 @@
         <v>2500</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>285</v>
@@ -452,6 +476,9 @@
       </c>
       <c r="I8" s="1" t="n">
         <v>100</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -459,7 +486,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>0</v>
@@ -471,7 +498,7 @@
         <v>2500</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>285</v>
@@ -481,6 +508,9 @@
       </c>
       <c r="I9" s="1" t="n">
         <v>100</v>
+      </c>
+      <c r="J9" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -488,7 +518,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>0</v>
@@ -500,7 +530,7 @@
         <v>2706</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G10" s="1" t="n">
         <v>80</v>
@@ -510,6 +540,9 @@
       </c>
       <c r="I10" s="1" t="n">
         <v>100</v>
+      </c>
+      <c r="J10" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -517,7 +550,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>0</v>
@@ -529,7 +562,7 @@
         <v>2683</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G11" s="1" t="n">
         <v>80</v>
@@ -540,10 +573,16 @@
       <c r="I11" s="1" t="n">
         <v>100</v>
       </c>
+      <c r="J11" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>